<commit_message>
updated script and files in csv instead of xlsx
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
   <si>
     <t xml:space="preserve">modelPath</t>
   </si>
@@ -118,91 +118,94 @@
     <t xml:space="preserve">measuredPrecision</t>
   </si>
   <si>
+    <t xml:space="preserve">/home/libotadmin/NewYork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tileset.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b6645aa5-4134-50f3-8cbc-faa0518c21bb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open-source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berkshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Som</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-04-26T07:09:20.560Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POINT(20.0924758 72.7341809)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDFMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cordoba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-emptive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cotton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iterate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cyan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deposit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tactics</t>
+  </si>
+  <si>
     <t xml:space="preserve">/tmp/tilesets/TilesetWithDiscreteLOD</t>
   </si>
   <si>
-    <t xml:space="preserve">tileset.json</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b6645aa5-4134-48f3-8cbc-faa0518c21bb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open-source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berkshire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Som</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-04-26T07:09:20.560Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POINT(20.0924758 72.7341809)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chicken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDFMU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cordoba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">white</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-emptive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cotton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">District</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iterate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cyan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deposit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tactics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc61d24d-7426-4490-a48f-06c13be98b85</t>
+    <t xml:space="preserve">Dc61d24d-7426-5090-a48f-06c13be98b85</t>
   </si>
   <si>
     <t xml:space="preserve">invoice</t>
@@ -268,7 +271,7 @@
     <t xml:space="preserve">monitor</t>
   </si>
   <si>
-    <t xml:space="preserve">deda97ad-0912-4524-929c-02beba91c01d</t>
+    <t xml:space="preserve">Deda97ad-0912-5024-929c-02beba91c01d</t>
   </si>
   <si>
     <t xml:space="preserve">portal</t>
@@ -425,7 +428,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -440,6 +443,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -523,10 +530,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -660,8 +667,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -685,13 +692,13 @@
       <c r="H2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -727,10 +734,10 @@
       <c r="V2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X2" s="4" t="s">
+      <c r="W2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>40</v>
       </c>
       <c r="Y2" s="3" t="s">
@@ -760,198 +767,296 @@
     </row>
     <row r="3" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="I3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>43</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="5" t="s">
         <v>40</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="4" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="4" t="s">
+      <c r="I4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>43</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="N5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="R4" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="Q5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="S5" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="W4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="3" t="s">
+      <c r="V5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="W5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="Z5" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AA5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AC4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AB5" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AC5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AE5" s="3" t="s">
         <v>100</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "updated script and files in csv instead of xlsx"
This reverts commit 90b68c702b6a11555e05a23cdd4ea7c9d6f34ff8.
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="101">
   <si>
     <t xml:space="preserve">modelPath</t>
   </si>
@@ -118,13 +118,13 @@
     <t xml:space="preserve">measuredPrecision</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/libotadmin/NewYork</t>
+    <t xml:space="preserve">/tmp/tilesets/TilesetWithDiscreteLOD</t>
   </si>
   <si>
     <t xml:space="preserve">tileset.json</t>
   </si>
   <si>
-    <t xml:space="preserve">b6645aa5-4134-50f3-8cbc-faa0518c21bb</t>
+    <t xml:space="preserve">b6645aa5-4134-48f3-8cbc-faa0518c21bb</t>
   </si>
   <si>
     <t xml:space="preserve">GB</t>
@@ -202,10 +202,7 @@
     <t xml:space="preserve">Tactics</t>
   </si>
   <si>
-    <t xml:space="preserve">/tmp/tilesets/TilesetWithDiscreteLOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dc61d24d-7426-5090-a48f-06c13be98b85</t>
+    <t xml:space="preserve">dc61d24d-7426-4490-a48f-06c13be98b85</t>
   </si>
   <si>
     <t xml:space="preserve">invoice</t>
@@ -271,7 +268,7 @@
     <t xml:space="preserve">monitor</t>
   </si>
   <si>
-    <t xml:space="preserve">Deda97ad-0912-5024-929c-02beba91c01d</t>
+    <t xml:space="preserve">deda97ad-0912-4524-929c-02beba91c01d</t>
   </si>
   <si>
     <t xml:space="preserve">portal</t>
@@ -428,7 +425,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -443,10 +440,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -530,10 +523,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -667,8 +660,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+    <row r="2" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -692,13 +685,13 @@
       <c r="H2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="I2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -734,10 +727,10 @@
       <c r="V2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="X2" s="5" t="s">
+      <c r="W2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="Y2" s="3" t="s">
@@ -767,296 +760,198 @@
     </row>
     <row r="3" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="5" t="s">
+      <c r="I3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>40</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>43</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="W3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AF3" s="3" t="s">
-        <v>82</v>
-      </c>
     </row>
-    <row r="4" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="5" t="s">
+      <c r="I4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>43</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="W4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="X4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD4" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="AC4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z5" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA5" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AE5" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>